<commit_message>
perubahan struktur data dosen dan program studi
</commit_message>
<xml_diff>
--- a/public/files/templates/Template_Dosen.xlsx
+++ b/public/files/templates/Template_Dosen.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Victus\Desktop\Asesmen-CPL\public\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58270CA-1CAF-4431-9ED7-D68457116037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A2EC7C-686F-4F81-A649-0E0967C41B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E794C9B1-78B5-4479-BF4F-91E9204B8E97}"/>
   </bookViews>
@@ -70,7 +70,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{0A715117-6F7E-4B96-8945-7A39BE6BDC1F}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B692AC77-9A23-4117-94D9-B75DBB1C2492}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Diisi dengan nama program studi yang terdaftar pada sistem.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{0A715117-6F7E-4B96-8945-7A39BE6BDC1F}">
       <text>
         <r>
           <rPr>
@@ -89,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Nama</t>
   </si>
@@ -125,13 +139,16 @@
   </si>
   <si>
     <t>P2MPP</t>
+  </si>
+  <si>
+    <t>Program Studi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +170,13 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -519,24 +543,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC493C55-F1BE-4C84-8128-E20F62FD170E}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="2" max="2" width="40.77734375" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="3" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="30.77734375" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" hidden="1"/>
+    <col min="5" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -556,13 +580,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="iDnODEPW2WWUERJEmy+IoKfpIR2aYwcCevwSIdBU9SMKq3qOApt+7YK7mbeAaPZLJxH6utsMe/OGPXo3nVywpg==" saltValue="5mkc6Q75HVOLFeCXuh/1Jg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="rxHPMDvI4j0CsWh4+5QpaD6O8K44P1jute/bImLVLfJO+ZmrNftYD7pRpOdMycLbmCvpVDEUI5uycGKCh7Y1cw==" saltValue="WiLKzxaKyLVD036T+X1Vhw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <protectedRanges>
-    <protectedRange sqref="A2:G1048576" name="Range1"/>
+    <protectedRange sqref="A2:H1048576" name="Range1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -580,7 +607,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G1048576</xm:sqref>
+          <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
fix fungsi halaman admin/dosen
</commit_message>
<xml_diff>
--- a/public/files/templates/Template_Dosen.xlsx
+++ b/public/files/templates/Template_Dosen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP Victus\Desktop\Asesmen-CPL\public\files\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89A2EC7C-686F-4F81-A649-0E0967C41B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAA9B58-6061-46B8-B30F-5A18D058C5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E794C9B1-78B5-4479-BF4F-91E9204B8E97}"/>
   </bookViews>
@@ -36,74 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>HP Victus</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{92881D37-EEBC-4F9A-90AD-6653BF7758B7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Diisi dengan "L" atau "P" tanpa tanda petik. Pilih melalui dropdown.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{63694D37-87A9-4D01-8EC9-A7909B95BF49}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Diisi dengan nama jurusan yang terdaftar pada sistem.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B692AC77-9A23-4117-94D9-B75DBB1C2492}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Diisi dengan nama program studi yang terdaftar pada sistem.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{0A715117-6F7E-4B96-8945-7A39BE6BDC1F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Diisi dengan "Dosen", "Koor. Program Studi" atau "P2MPP" tanpa tanda petik. Pilih melalui dropdown.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Nama</t>
   </si>
@@ -148,7 +82,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,30 +98,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -195,20 +121,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,7 +487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC493C55-F1BE-4C84-8128-E20F62FD170E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC493C55-F1BE-4C84-8128-E20F62FD170E}">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
@@ -551,49 +496,46 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.77734375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="40.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" style="3" customWidth="1"/>
-    <col min="5" max="7" width="30.77734375" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="40.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="6" customWidth="1"/>
+    <col min="5" max="7" width="30.77734375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" hidden="1" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="H1" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rxHPMDvI4j0CsWh4+5QpaD6O8K44P1jute/bImLVLfJO+ZmrNftYD7pRpOdMycLbmCvpVDEUI5uycGKCh7Y1cw==" saltValue="WiLKzxaKyLVD036T+X1Vhw==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FL0AhQcqrH+fyjoFsXkB7bzU2XY2cRztrJqrYYVHHSxht33+l5L/3yYeMGkA7tRR1HQNQnIsXRqf8gCdUVCxAA==" saltValue="glUzJgzBOyIUCkcYZN2U/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
   <protectedRanges>
-    <protectedRange sqref="A2:H1048576" name="Range1"/>
+    <protectedRange sqref="A2:G1048576" name="Range1"/>
   </protectedRanges>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">

</xml_diff>